<commit_message>
Contact number ralated changes
</commit_message>
<xml_diff>
--- a/ExternalData/QuestionTestData.xlsx
+++ b/ExternalData/QuestionTestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>Akila</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>Akila.Theekshana#@gmail,com</t>
+  </si>
+  <si>
+    <t>Akila.Theekshana@gmail.com</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>71-5465877</t>
   </si>
 </sst>
 </file>
@@ -184,12 +193,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -717,10 +729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,9 +740,10 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -740,8 +753,11 @@
       <c r="C1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -749,17 +765,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -767,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -775,7 +791,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -783,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -791,7 +807,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -802,7 +818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -813,18 +829,61 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>715465977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1"/>
     <hyperlink ref="C10" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C13" r:id="rId4"/>
+    <hyperlink ref="C14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>